<commit_message>
Final na ba i2
</commit_message>
<xml_diff>
--- a/Admin/exported_data.xlsx
+++ b/Admin/exported_data.xlsx
@@ -518,20 +518,16 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
+      <c r="B2"/>
+      <c r="C2"/>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -544,7 +540,7 @@
       </c>
       <c r="J2"/>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -612,17 +608,13 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
+      <c r="B4"/>
+      <c r="C4"/>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -634,14 +626,14 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4"/>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -797,7 +789,7 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1026,16 +1018,16 @@
         <v>28</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1044,14 +1036,14 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13"/>
       <c r="K13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1119,20 +1111,16 @@
       <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
+      <c r="B15"/>
+      <c r="C15"/>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1145,7 +1133,7 @@
       </c>
       <c r="J15"/>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1214,35 +1202,35 @@
         <v>32</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17"/>
       <c r="K17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <v>0</v>

</xml_diff>